<commit_message>
changed how I define z score in the network plot to make it more reasonable
</commit_message>
<xml_diff>
--- a/Stim info.xlsx
+++ b/Stim info.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Pt1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Pt2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Pt3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Pt4" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="162">
   <si>
     <t>Ieeg name</t>
   </si>
@@ -30,7 +31,7 @@
     <t>Electrodes</t>
   </si>
   <si>
-    <t>Stim seizure elecs</t>
+    <t>Clinical Stim seizure elecs</t>
   </si>
   <si>
     <t>Suspected SOZ anatomic</t>
@@ -424,6 +425,81 @@
   </si>
   <si>
     <t>RB9</t>
+  </si>
+  <si>
+    <t>LM3</t>
+  </si>
+  <si>
+    <t>LA1 and LA2: weird cephalic feeling</t>
+  </si>
+  <si>
+    <t>Looks like nice cceps LC6-&gt;LB9; LA1-&gt;LC1;LA2-&gt;LL1;LJ3-&gt;LH5</t>
+  </si>
+  <si>
+    <t>LA2</t>
+  </si>
+  <si>
+    <t>LD8</t>
+  </si>
+  <si>
+    <t>LA3</t>
+  </si>
+  <si>
+    <t>LD9</t>
+  </si>
+  <si>
+    <t>left mid cingulate</t>
+  </si>
+  <si>
+    <t>LL1</t>
+  </si>
+  <si>
+    <t>left parietal MEG dipole</t>
+  </si>
+  <si>
+    <t>LL2</t>
+  </si>
+  <si>
+    <t>left SMA</t>
+  </si>
+  <si>
+    <t>LL3</t>
+  </si>
+  <si>
+    <t>left frontal eye field</t>
+  </si>
+  <si>
+    <t>left superior frontal gyrus</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>left frontal pole</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>left orbitofrontal gyrus</t>
+  </si>
+  <si>
+    <t>LC8</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>LB3</t>
+  </si>
+  <si>
+    <t>LB9</t>
+  </si>
+  <si>
+    <t>LB10</t>
+  </si>
+  <si>
+    <t>LJ4</t>
   </si>
 </sst>
 </file>
@@ -483,6 +559,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -706,7 +786,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -727,7 +807,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -835,7 +915,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -856,7 +936,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -870,10 +950,10 @@
       <c r="B2" s="1">
         <v>3.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>18893.11</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>21999.75</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1047,27 +1127,27 @@
       </c>
     </row>
     <row r="23">
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25">
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26">
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="27">
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1217,7 +1297,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1238,7 +1318,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1570,4 +1650,340 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="E3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="E6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="E7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="E8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="E10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="E13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code to port to other servers
</commit_message>
<xml_diff>
--- a/Stim info.xlsx
+++ b/Stim info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="164">
   <si>
     <t>Ieeg name</t>
   </si>
@@ -304,6 +304,9 @@
     <t>LJ3</t>
   </si>
   <si>
+    <t>HUP214_CCEP</t>
+  </si>
+  <si>
     <t>Bilateral mesial temporal</t>
   </si>
   <si>
@@ -425,6 +428,9 @@
   </si>
   <si>
     <t>RB9</t>
+  </si>
+  <si>
+    <t>HUP213_CCEP</t>
   </si>
   <si>
     <t>LM3</t>
@@ -1326,12 +1332,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="B2" s="1">
         <v>1.0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="2">
+        <v>7086.47</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9048.39</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
@@ -1339,10 +1351,10 @@
         <v>58</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>35</v>
@@ -1359,7 +1371,7 @@
         <v>16</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>38</v>
@@ -1373,7 +1385,7 @@
         <v>69</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>41</v>
@@ -1384,7 +1396,7 @@
     </row>
     <row r="5">
       <c r="E5" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>44</v>
@@ -1395,7 +1407,7 @@
     </row>
     <row r="6">
       <c r="E6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>47</v>
@@ -1423,7 +1435,7 @@
         <v>18</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
@@ -1445,7 +1457,7 @@
         <v>57</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11">
@@ -1453,32 +1465,32 @@
         <v>92</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="E12" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="E13" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14">
@@ -1486,10 +1498,10 @@
         <v>32</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15">
@@ -1497,10 +1509,10 @@
         <v>37</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16">
@@ -1516,13 +1528,13 @@
     </row>
     <row r="17">
       <c r="E17" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18">
@@ -1530,7 +1542,7 @@
         <v>58</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>26</v>
@@ -1538,63 +1550,63 @@
     </row>
     <row r="19">
       <c r="E19" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20">
       <c r="E20" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21">
       <c r="E21" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22">
       <c r="E22" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23">
       <c r="E23" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
       <c r="E24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
       <c r="E25" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26">
       <c r="E26" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27">
       <c r="E27" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">
       <c r="E28" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">
       <c r="E29" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
@@ -1604,27 +1616,27 @@
     </row>
     <row r="31">
       <c r="E31" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32">
       <c r="E32" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33">
       <c r="E33" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34">
       <c r="E34" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
       <c r="E35" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36">
@@ -1634,17 +1646,17 @@
     </row>
     <row r="37">
       <c r="E37" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38">
       <c r="E38" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39">
       <c r="E39" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1707,11 +1719,20 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="B2" s="1">
         <v>3.0</v>
       </c>
+      <c r="C2" s="1">
+        <v>13215.01</v>
+      </c>
+      <c r="D2" s="1">
+        <v>15445.34</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>93</v>
@@ -1720,10 +1741,10 @@
         <v>58</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>35</v>
@@ -1732,7 +1753,7 @@
         <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
@@ -1774,21 +1795,21 @@
         <v>63</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
       <c r="E6" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>47</v>
@@ -1799,7 +1820,7 @@
     </row>
     <row r="7">
       <c r="E7" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>82</v>
@@ -1808,40 +1829,40 @@
         <v>22</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8">
       <c r="E8" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9">
       <c r="E9" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10">
       <c r="E10" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>57</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11">
@@ -1852,7 +1873,7 @@
         <v>59</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12">
@@ -1860,29 +1881,29 @@
         <v>49</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13">
       <c r="E13" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14">
       <c r="E14" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>19</v>
@@ -1900,17 +1921,17 @@
     </row>
     <row r="17">
       <c r="E17" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18">
       <c r="E18" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19">
       <c r="E19" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
@@ -1920,27 +1941,27 @@
     </row>
     <row r="21">
       <c r="E21" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22">
       <c r="E22" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23">
       <c r="E23" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24">
       <c r="E24" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25">
       <c r="E25" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26">

</xml_diff>

<commit_message>
ability to loop through times
</commit_message>
<xml_diff>
--- a/Stim info.xlsx
+++ b/Stim info.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="Pt2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Pt3" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Pt4" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Pt5" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="167">
   <si>
     <t>Ieeg name</t>
   </si>
@@ -28,6 +29,9 @@
     <t>Main stim end time</t>
   </si>
   <si>
+    <t>Time breaks</t>
+  </si>
+  <si>
     <t>Electrodes</t>
   </si>
   <si>
@@ -506,6 +510,12 @@
   </si>
   <si>
     <t>LJ4</t>
+  </si>
+  <si>
+    <t>CHOP_CCEPs</t>
+  </si>
+  <si>
+    <t>3 mA</t>
   </si>
 </sst>
 </file>
@@ -569,6 +579,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -789,10 +803,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -819,10 +833,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>3.0</v>
@@ -833,61 +850,62 @@
       <c r="D2" s="1">
         <v>13592.42</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3">
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4">
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5">
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6">
-      <c r="E6" s="1" t="s">
-        <v>30</v>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -918,10 +936,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -948,10 +966,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>3.0</v>
@@ -962,314 +983,315 @@
       <c r="D2" s="1">
         <v>21999.75</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3">
-      <c r="E3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4">
-      <c r="E4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5">
-      <c r="E5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6">
-      <c r="E6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7">
-      <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>22</v>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>50</v>
+        <v>23</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8">
-      <c r="E8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>18</v>
+      <c r="F8" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9">
-      <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="N9" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10">
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>57</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>59</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12">
-      <c r="E12" s="1" t="s">
-        <v>34</v>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13">
-      <c r="E13" s="1" t="s">
-        <v>61</v>
+      <c r="F13" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14">
-      <c r="E14" s="1" t="s">
-        <v>62</v>
+      <c r="F14" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15">
-      <c r="E15" s="1" t="s">
-        <v>63</v>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="16">
-      <c r="E16" s="1" t="s">
-        <v>64</v>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17">
-      <c r="E17" s="1" t="s">
-        <v>65</v>
+      <c r="F17" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18">
-      <c r="E18" s="1" t="s">
-        <v>66</v>
+      <c r="F18" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19">
-      <c r="E19" s="1" t="s">
-        <v>67</v>
+      <c r="F19" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20">
-      <c r="E20" s="1" t="s">
-        <v>68</v>
+      <c r="F20" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21">
-      <c r="E21" s="1" t="s">
-        <v>69</v>
+      <c r="F21" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22">
-      <c r="E22" s="1" t="s">
-        <v>70</v>
+      <c r="F22" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23">
-      <c r="E23" s="1" t="s">
-        <v>24</v>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="1" t="s">
-        <v>71</v>
+      <c r="F24" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25">
-      <c r="E25" s="1" t="s">
-        <v>72</v>
+      <c r="F25" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26">
-      <c r="E26" s="1" t="s">
-        <v>73</v>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27">
-      <c r="E27" s="1" t="s">
-        <v>74</v>
+      <c r="F27" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28">
-      <c r="E28" s="1" t="s">
-        <v>15</v>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29">
-      <c r="E29" s="1" t="s">
-        <v>20</v>
+      <c r="F29" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30">
-      <c r="E30" s="1" t="s">
-        <v>75</v>
+      <c r="F30" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31">
-      <c r="E31" s="1" t="s">
-        <v>76</v>
+      <c r="F31" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32">
-      <c r="E32" s="1" t="s">
-        <v>77</v>
+      <c r="F32" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="33">
-      <c r="E33" s="1" t="s">
-        <v>78</v>
+      <c r="F33" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="34">
-      <c r="E34" s="1" t="s">
-        <v>79</v>
+      <c r="F34" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="35">
-      <c r="E35" s="1" t="s">
-        <v>80</v>
+      <c r="F35" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="36">
-      <c r="E36" s="1" t="s">
-        <v>81</v>
+      <c r="F36" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="37">
-      <c r="E37" s="1" t="s">
-        <v>82</v>
+      <c r="F37" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38">
-      <c r="E38" s="1" t="s">
-        <v>83</v>
+      <c r="F38" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="39">
-      <c r="E39" s="1" t="s">
-        <v>84</v>
+      <c r="F39" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="40">
-      <c r="E40" s="1" t="s">
-        <v>85</v>
+      <c r="F40" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41">
-      <c r="E41" s="1" t="s">
-        <v>86</v>
+      <c r="F41" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="42">
-      <c r="E42" s="1" t="s">
-        <v>87</v>
+      <c r="F42" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="43">
-      <c r="E43" s="1" t="s">
-        <v>88</v>
+      <c r="F43" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="44">
-      <c r="E44" s="1" t="s">
-        <v>89</v>
+      <c r="F44" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="45">
-      <c r="E45" s="1" t="s">
-        <v>90</v>
+      <c r="F45" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46">
-      <c r="E46" s="1" t="s">
-        <v>91</v>
+      <c r="F46" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="47">
-      <c r="E47" s="1" t="s">
-        <v>92</v>
+      <c r="F47" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="48">
-      <c r="E48" s="1" t="s">
-        <v>93</v>
+      <c r="F48" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="49">
-      <c r="E49" s="1" t="s">
-        <v>94</v>
+      <c r="F49" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="50">
-      <c r="E50" s="1" t="s">
-        <v>95</v>
+      <c r="F50" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1300,10 +1322,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1330,333 +1352,337 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>96</v>
+      <c r="A2" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="B2" s="1">
         <v>1.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>7086.47</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>9048.39</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>98</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3">
-      <c r="E3" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>99</v>
+        <v>68</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4">
-      <c r="E4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>100</v>
+      <c r="F4" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5">
-      <c r="E5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>44</v>
+      <c r="F5" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6">
-      <c r="E6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>47</v>
+      <c r="F6" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7">
-      <c r="E7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>22</v>
+      <c r="F7" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8">
-      <c r="E8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>18</v>
+      <c r="F8" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>102</v>
+        <v>19</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9">
-      <c r="E9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>54</v>
+      <c r="F9" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10">
-      <c r="E10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>57</v>
+      <c r="F10" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="11">
-      <c r="E11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>104</v>
+      <c r="F11" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="12">
-      <c r="E12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>107</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="13">
-      <c r="E13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>110</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="N13" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14">
-      <c r="E14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>112</v>
+      <c r="F14" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="15">
-      <c r="E15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>114</v>
+      <c r="F15" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="N15" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="16">
-      <c r="E16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>28</v>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N16" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17">
-      <c r="E17" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>25</v>
+      <c r="F17" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>117</v>
+        <v>26</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18">
-      <c r="E18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>118</v>
+      <c r="F18" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>26</v>
+        <v>119</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19">
-      <c r="E19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>120</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="N19" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="20">
-      <c r="E20" s="1" t="s">
-        <v>122</v>
+      <c r="F20" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21">
-      <c r="E21" s="1" t="s">
-        <v>123</v>
+      <c r="F21" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="22">
-      <c r="E22" s="1" t="s">
-        <v>124</v>
+      <c r="F22" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="23">
-      <c r="E23" s="1" t="s">
-        <v>99</v>
+      <c r="F23" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="1" t="s">
-        <v>125</v>
+      <c r="F24" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25">
-      <c r="E25" s="1" t="s">
-        <v>126</v>
+      <c r="F25" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26">
-      <c r="E26" s="1" t="s">
-        <v>127</v>
+      <c r="F26" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="27">
-      <c r="E27" s="1" t="s">
-        <v>128</v>
+      <c r="F27" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="28">
-      <c r="E28" s="1" t="s">
-        <v>129</v>
+      <c r="F28" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="29">
-      <c r="E29" s="1" t="s">
-        <v>130</v>
+      <c r="F29" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="30">
-      <c r="E30" s="1" t="s">
-        <v>21</v>
+      <c r="F30" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="31">
-      <c r="E31" s="1" t="s">
-        <v>131</v>
+      <c r="F31" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="32">
-      <c r="E32" s="1" t="s">
-        <v>132</v>
+      <c r="F32" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="33">
-      <c r="E33" s="1" t="s">
-        <v>133</v>
+      <c r="F33" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34">
-      <c r="E34" s="1" t="s">
-        <v>134</v>
+      <c r="F34" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="35">
-      <c r="E35" s="1" t="s">
-        <v>135</v>
+      <c r="F35" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="36">
-      <c r="E36" s="1" t="s">
-        <v>16</v>
+      <c r="F36" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="37">
-      <c r="E37" s="1" t="s">
-        <v>136</v>
+      <c r="F37" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="38">
-      <c r="E38" s="1" t="s">
-        <v>137</v>
+      <c r="F38" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="39">
-      <c r="E39" s="1" t="s">
-        <v>100</v>
+      <c r="F39" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1687,10 +1713,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1717,10 +1743,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>138</v>
+      <c r="A2" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="B2" s="1">
         <v>3.0</v>
@@ -1731,277 +1760,410 @@
       <c r="D2" s="1">
         <v>15445.34</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>58</v>
+        <v>140</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>141</v>
+        <v>37</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3">
-      <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4">
-      <c r="E4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>41</v>
+      <c r="F4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5">
-      <c r="E5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>44</v>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>103</v>
+        <v>45</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6">
-      <c r="E6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="F7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="F9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="F10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="F11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="E7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="E8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="E9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="E10" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>153</v>
+        <v>60</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="12">
-      <c r="E12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>154</v>
+      <c r="F12" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="13">
-      <c r="E13" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>156</v>
+      <c r="F13" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="N13" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="14">
-      <c r="E14" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>159</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>19</v>
+        <v>160</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15">
-      <c r="E15" s="2" t="s">
-        <v>58</v>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16">
-      <c r="E16" s="2" t="s">
-        <v>34</v>
+      <c r="F16" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17">
-      <c r="E17" s="2" t="s">
-        <v>160</v>
+      <c r="F17" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18">
-      <c r="E18" s="2" t="s">
-        <v>161</v>
+      <c r="F18" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="19">
-      <c r="E19" s="2" t="s">
-        <v>162</v>
+      <c r="F19" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="20">
-      <c r="E20" s="2" t="s">
-        <v>51</v>
+      <c r="F20" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21">
-      <c r="E21" s="2" t="s">
-        <v>142</v>
+      <c r="F21" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="22">
-      <c r="E22" s="2" t="s">
-        <v>144</v>
+      <c r="F22" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="23">
-      <c r="E23" s="2" t="s">
-        <v>124</v>
+      <c r="F23" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="24">
-      <c r="E24" s="2" t="s">
-        <v>99</v>
+      <c r="F24" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="25">
-      <c r="E25" s="2" t="s">
-        <v>163</v>
+      <c r="F25" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="26">
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="F27" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27">
-      <c r="E27" s="2" t="s">
+    <row r="28">
+      <c r="F28" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="F29" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="F30" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28">
-      <c r="E28" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="E29" s="2" t="s">
+    <row r="31">
+      <c r="F31" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30">
-      <c r="E30" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="E31" s="2" t="s">
+    <row r="32">
+      <c r="F32" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32">
-      <c r="E32" s="1" t="s">
+    <row r="33">
+      <c r="F33" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33">
-      <c r="E33" s="1" t="s">
-        <v>78</v>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="1">
+        <v>170.95</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9347.8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>170.95</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="E3" s="1">
+        <v>1051.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" s="2">
+        <v>2168.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="E5" s="1">
+        <v>3099.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="E6" s="1">
+        <v>4031.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="E7" s="1">
+        <v>4978.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="E8" s="1">
+        <v>6110.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" s="1">
+        <v>7027.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="E10" s="1">
+        <v>8031.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" s="1">
+        <v>8806.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" s="1">
+        <v>9347.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>